<commit_message>
table 1 output in excel
</commit_message>
<xml_diff>
--- a/analysis/output/table1.xlsx
+++ b/analysis/output/table1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,6 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -141,6 +140,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,7 +478,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection sqref="A1:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -488,196 +490,205 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" ht="17">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>0</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>1</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>5</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>10</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>20</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>40</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>60</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <v>80</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="5">
         <v>90</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="5">
         <v>95</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="5">
         <v>99</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="5">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="17">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>-1085548.6359999999</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>0</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>0</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>0</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>3753.7663108000002</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>30435.943060000001</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
         <v>63915.480427399998</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
         <v>152179.71530000001</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="6">
         <v>486975.08896999998</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="6">
         <v>1374690.0948999999</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="7">
         <v>9424997.0343900006</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="6">
         <v>154929095.49419999</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="17">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>0</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>7101.7200474000001</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>12174.377224</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>17247.034401000001</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>26489.415776999998</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>50726.571767000001</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>86235.172005</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="6">
         <v>193775.50414999999</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="6">
         <v>699012.15896000003</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <v>2242114.4720999999</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="6">
         <v>12072416.81525</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="6">
         <v>179937295.37</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="17">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>-227019000</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>-74425</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>-14367.5</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>-130</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>6400</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>66600</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>294850</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="8">
         <v>1603900</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <v>9602000</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="8">
         <v>33258525</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="8">
         <v>176453425</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="8">
         <v>1324417600</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>